<commit_message>
Fix FRAN CSV import: Handle semicolon delimiter, European number format, _FINAL_OUTPUT suffix, and comma-separated DocNumbers
</commit_message>
<xml_diff>
--- a/data/fran_consolidated.xlsx
+++ b/data/fran_consolidated.xlsx
@@ -16,7 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +512,906 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1050D</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>58</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>45967.79786944447</v>
+      </c>
+      <c r="N2" t="n">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>570BE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>137</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>45967.79945715976</v>
+      </c>
+      <c r="N3" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1450I</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>GBP2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>51</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>45967.79808251436</v>
+      </c>
+      <c r="N4" t="n">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CIT01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>OP272</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>45967.79807569226</v>
+      </c>
+      <c r="N5" t="n">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1850I</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>28</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>45967.79796980104</v>
+      </c>
+      <c r="N6" t="n">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1939I</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>45967.79732171625</v>
+      </c>
+      <c r="N7" t="n">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2439I</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NOK_2</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>13</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>45967.79861421794</v>
+      </c>
+      <c r="N8" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2602D</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PLN</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>37</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3" t="n">
+        <v>45967.7997921789</v>
+      </c>
+      <c r="N9" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3350I</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>93</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3" t="n">
+        <v>45967.79917160589</v>
+      </c>
+      <c r="N10" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3350I</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>45967.79901506098</v>
+      </c>
+      <c r="N11" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4050I</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>45</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>45967.79893278747</v>
+      </c>
+      <c r="N12" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SAN01</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>OP464</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>359</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3" t="n">
+        <v>45967.9241951217</v>
+      </c>
+      <c r="N13" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4150I</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>66</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3" t="n">
+        <v>45967.79996921462</v>
+      </c>
+      <c r="N14" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4175I</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>16</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3" t="n">
+        <v>45967.80016350422</v>
+      </c>
+      <c r="N15" t="n">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4234D</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>97</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3" t="n">
+        <v>45967.80013625809</v>
+      </c>
+      <c r="N16" t="n">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>4335I</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3" t="n">
+        <v>45967.8001032894</v>
+      </c>
+      <c r="N17" t="n">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4350I</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>122</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3" t="n">
+        <v>45967.80100663648</v>
+      </c>
+      <c r="N18" t="n">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4450I</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CZK</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>14</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3" t="n">
+        <v>45967.80043785644</v>
+      </c>
+      <c r="N19" t="n">
+        <v>672</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix FRAN CSV parsing: Use comma delimiter with quoted fields and proper US number format conversion
</commit_message>
<xml_diff>
--- a/data/fran_consolidated.xlsx
+++ b/data/fran_consolidated.xlsx
@@ -535,25 +535,25 @@
         <v>58</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>817382.7100000001</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>817382.7100000001</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>430067.28</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>430067.28</v>
       </c>
       <c r="M2" s="3" t="n">
         <v>45967.79786944447</v>
@@ -585,25 +585,25 @@
         <v>137</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>887627.22</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>887627.22</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>325272.0600000001</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>325272.0600000001</v>
       </c>
       <c r="M3" s="3" t="n">
         <v>45967.79945715976</v>
@@ -635,25 +635,25 @@
         <v>51</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>8173894.139999999</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>9563456.143799998</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>691057.36</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>808537.1111999999</v>
       </c>
       <c r="M4" s="3" t="n">
         <v>45967.79808251436</v>
@@ -685,25 +685,25 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>33735.12</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>33735.12</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>4096.1</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>4096.1</v>
       </c>
       <c r="M5" s="3" t="n">
         <v>45967.79807569226</v>
@@ -735,25 +735,25 @@
         <v>28</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2520978.8</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>2520978.8</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>58858.24000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>58858.24000000001</v>
       </c>
       <c r="M6" s="3" t="n">
         <v>45967.79796980104</v>
@@ -785,25 +785,25 @@
         <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>87712.25999999999</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>87712.25999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1420.71</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1420.71</v>
       </c>
       <c r="M7" s="3" t="n">
         <v>45967.79732171625</v>
@@ -835,25 +835,25 @@
         <v>13</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>11601121.53</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>974494.2085199999</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>57023.46</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>4789.97064</v>
       </c>
       <c r="M8" s="3" t="n">
         <v>45967.79861421794</v>
@@ -885,25 +885,25 @@
         <v>37</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>649469.88</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>149378.0724</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>48199.26</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>11085.8298</v>
       </c>
       <c r="M9" s="3" t="n">
         <v>45967.7997921789</v>
@@ -935,25 +935,25 @@
         <v>93</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>5018728.44</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>5018728.44</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1308416.98</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>1308416.98</v>
       </c>
       <c r="M10" s="3" t="n">
         <v>45967.79917160589</v>
@@ -985,25 +985,25 @@
         <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>230011.68</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>211610.7456</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>149673.18</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>137699.3256</v>
       </c>
       <c r="M11" s="3" t="n">
         <v>45967.79901506098</v>
@@ -1035,25 +1035,25 @@
         <v>45</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1344304.89</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1344304.89</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>663.23</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>663.23</v>
       </c>
       <c r="M12" s="3" t="n">
         <v>45967.79893278747</v>
@@ -1085,25 +1085,25 @@
         <v>359</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>353588.11</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>353588.11</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>359</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>6489.45</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>6489.45</v>
       </c>
       <c r="M13" s="3" t="n">
         <v>45967.9241951217</v>
@@ -1135,25 +1135,25 @@
         <v>66</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>5888894.439999999</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>5888894.439999999</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>112453.05</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>112453.05</v>
       </c>
       <c r="M14" s="3" t="n">
         <v>45967.79996921462</v>
@@ -1185,25 +1185,25 @@
         <v>16</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>204386.29</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>204386.29</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>11429.92</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>11429.92</v>
       </c>
       <c r="M15" s="3" t="n">
         <v>45967.80016350422</v>
@@ -1235,16 +1235,16 @@
         <v>97</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>2333841.4</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2333841.4</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1285,25 +1285,25 @@
         <v>8</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>129593.76</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>129593.76</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>918.2</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>918.2</v>
       </c>
       <c r="M17" s="3" t="n">
         <v>45967.8001032894</v>
@@ -1335,25 +1335,25 @@
         <v>122</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>7177062.160000001</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>7177062.160000001</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>474741.27</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>474741.27</v>
       </c>
       <c r="M18" s="3" t="n">
         <v>45967.80100663648</v>
@@ -1385,25 +1385,25 @@
         <v>14</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>2659261</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>103711.179</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>500526.8700000001</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>19520.54793</v>
       </c>
       <c r="M19" s="3" t="n">
         <v>45967.80043785644</v>

</xml_diff>